<commit_message>
Consultas realizadas el 25 de septiembre
</commit_message>
<xml_diff>
--- a/Cargas Masivas.xlsx
+++ b/Cargas Masivas.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="185">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
@@ -522,6 +522,9 @@
     <t xml:space="preserve">PEV</t>
   </si>
   <si>
+    <t xml:space="preserve">Tecnico en Administracion de Empresas - Negocios</t>
+  </si>
+  <si>
     <t xml:space="preserve">TLP</t>
   </si>
   <si>
@@ -534,9 +537,6 @@
     <t xml:space="preserve">escuela_id</t>
   </si>
   <si>
-    <t xml:space="preserve">empleado_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">Carrera-Escuela</t>
   </si>
   <si>
@@ -552,10 +552,37 @@
     <t xml:space="preserve">INF001</t>
   </si>
   <si>
+    <t xml:space="preserve">Tecnologia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecnico en Administracion de Empresas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAD0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negocios</t>
+  </si>
+  <si>
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">Bellavista</t>
+    <t xml:space="preserve">Auditoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUD0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingenieria en Negocios Electronicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INE0001</t>
   </si>
 </sst>
 </file>
@@ -572,6 +599,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -593,6 +621,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -643,7 +672,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -652,7 +681,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -661,6 +690,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -699,7 +732,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.84"/>
@@ -961,14 +994,14 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D15" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D15" type="list">
       <formula1>Regiones!$A$2:$A$17</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -987,7 +1020,7 @@
       <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="55.73"/>
@@ -1023,11 +1056,11 @@
       <c r="B2" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D2,Regiones!A:C,3,0),"")</f>
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -1048,11 +1081,11 @@
       <c r="B3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D3,Regiones!A:C,3,0),"")</f>
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="0" t="n">
@@ -1073,11 +1106,11 @@
       <c r="B4" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D4,Regiones!A:C,3,0),"")</f>
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="0" t="n">
@@ -1098,11 +1131,11 @@
       <c r="B5" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D5,Regiones!A:C,3,0),"")</f>
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E5" s="0" t="n">
@@ -1123,11 +1156,11 @@
       <c r="B6" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D6,Regiones!A:C,3,0),"")</f>
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="0" t="n">
@@ -1148,11 +1181,11 @@
       <c r="B7" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D7,Regiones!A:C,3,0),"")</f>
         <v>16</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="0" t="n">
@@ -1173,11 +1206,11 @@
       <c r="B8" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D8,Regiones!A:C,3,0),"")</f>
         <v>15</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="0" t="n">
@@ -1198,11 +1231,11 @@
       <c r="B9" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D9,Regiones!A:C,3,0),"")</f>
         <v>4</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="0" t="n">
@@ -1223,11 +1256,11 @@
       <c r="B10" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D10,Regiones!A:C,3,0),"")</f>
         <v>1</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="0" t="n">
@@ -1248,11 +1281,11 @@
       <c r="B11" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D11,Regiones!A:C,3,0),"")</f>
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="0" t="n">
@@ -1273,11 +1306,11 @@
       <c r="B12" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D12,Regiones!A:C,3,0),"")</f>
         <v>8</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="0" t="n">
@@ -1298,11 +1331,11 @@
       <c r="B13" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D13,Regiones!A:C,3,0),"")</f>
         <v>10</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="0" t="n">
@@ -1323,11 +1356,11 @@
       <c r="B14" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D14,Regiones!A:C,3,0),"")</f>
         <v>4</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="0" t="n">
@@ -1348,11 +1381,11 @@
       <c r="B15" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D15,Regiones!A:C,3,0),"")</f>
         <v>16</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="0" t="n">
@@ -1373,11 +1406,11 @@
       <c r="B16" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D16,Regiones!A:C,3,0),"")</f>
         <v>4</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E16" s="0" t="n">
@@ -1398,11 +1431,11 @@
       <c r="B17" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="C17" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D17,Regiones!A:C,3,0),"")</f>
         <v>1</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E17" s="0" t="n">
@@ -1423,11 +1456,11 @@
       <c r="B18" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D18,Regiones!A:C,3,0),"")</f>
         <v>2</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E18" s="0" t="n">
@@ -1448,11 +1481,11 @@
       <c r="B19" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="C19" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D19,Regiones!A:C,3,0),"")</f>
         <v>2</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E19" s="0" t="n">
@@ -1473,11 +1506,11 @@
       <c r="B20" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="C20" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D20,Regiones!A:C,3,0),"")</f>
         <v>4</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="0" t="n">
@@ -1498,11 +1531,11 @@
       <c r="B21" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="C21" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D21,Regiones!A:C,3,0),"")</f>
         <v>3</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E21" s="0" t="n">
@@ -1523,11 +1556,11 @@
       <c r="B22" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="C22" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D22,Regiones!A:C,3,0),"")</f>
         <v>1</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="0" t="n">
@@ -1548,11 +1581,11 @@
       <c r="B23" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="2" t="n">
+      <c r="C23" s="1" t="n">
         <f aca="false">IFERROR(VLOOKUP(D23,Regiones!A:C,3,0),"")</f>
         <v>1</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E23" s="0" t="n">
@@ -1565,14 +1598,14 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D23" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D23" type="list">
       <formula1>Regiones!$A$2:$A$17</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -1591,7 +1624,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
   </cols>
@@ -1654,7 +1687,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -1673,7 +1706,7 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="33.29"/>
   </cols>
@@ -1750,9 +1783,9 @@
       <c r="J2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="0" t="str">
+      <c r="K2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(C2," - ",I2)</f>
-        <v>Pablo Contreras -  Director(a) de Sede    </v>
+        <v>Pablo Contreras -  Director(a) de Sede</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>1</v>
@@ -1793,9 +1826,9 @@
       <c r="J3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="0" t="str">
+      <c r="K3" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(C3," - ",I3)</f>
-        <v>Laura Diaz -  Director(a) de Escuela </v>
+        <v>Laura Diaz -  Director(a) de Escuela</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>2</v>
@@ -1836,7 +1869,7 @@
       <c r="J4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="0" t="str">
+      <c r="K4" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(C4," - ",I4)</f>
         <v>Luis Mora -  Jefe(a) de Carrera</v>
       </c>
@@ -1879,9 +1912,9 @@
       <c r="J5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="0" t="str">
+      <c r="K5" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(C5," - ",I5)</f>
-        <v>Javiera Rosales -  Director(a) de Sede    </v>
+        <v>Javiera Rosales -  Director(a) de Sede</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>4</v>
@@ -1922,9 +1955,9 @@
       <c r="J6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="0" t="str">
+      <c r="K6" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(C6," - ",I6)</f>
-        <v>Lucia Suarez -  Director(a) de Escuela </v>
+        <v>Lucia Suarez -  Director(a) de Escuela</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>5</v>
@@ -1947,7 +1980,7 @@
       <c r="D7" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>101</v>
       </c>
       <c r="F7" s="0" t="s">
@@ -1967,9 +2000,9 @@
       <c r="J7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="0" t="str">
+      <c r="K7" s="5" t="str">
         <f aca="false">_xlfn.CONCAT(C7," - ",I7)</f>
-        <v>Luis Ramirez -  Director(a) de Sede    </v>
+        <v>Luis Ramirez -  Director(a) de Sede</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>6</v>
@@ -2017,15 +2050,15 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I19" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I19" type="list">
       <formula1>roles!$B$2:$B$10</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J7" type="list">
       <formula1>Comunas!$B$2:$B$40</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K2:K7" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K2:K7" type="none">
       <formula1>Comunas!$B$2:$B$40</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2035,7 +2068,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -2054,14 +2087,14 @@
       <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -2076,7 +2109,7 @@
       <c r="E1" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>61</v>
       </c>
       <c r="G1" s="0" t="s">
@@ -2090,7 +2123,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
+      <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -2105,7 +2138,7 @@
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="7" t="n">
         <v>1</v>
       </c>
       <c r="I2" s="0" t="str">
@@ -2114,7 +2147,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
+      <c r="A3" s="7" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -2129,7 +2162,7 @@
       <c r="E3" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="7" t="n">
         <v>2</v>
       </c>
       <c r="I3" s="0" t="str">
@@ -2152,10 +2185,10 @@
         <f aca="false">VLOOKUP(H4,Empleados!K:L,2,0)</f>
         <v>6</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="4" t="s">
         <v>112</v>
       </c>
       <c r="I4" s="0" t="str">
@@ -2165,18 +2198,18 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G4" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G4" type="list">
       <formula1>Comunas!$B$2:$B$40</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H4" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H4" type="list">
       <formula1>Empleados!$K$2:$K$42</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -2195,7 +2228,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="55.52"/>
   </cols>
@@ -2364,7 +2397,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -2383,7 +2416,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="121.25"/>
   </cols>
@@ -2433,7 +2466,7 @@
       <c r="D2" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>137</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -2467,7 +2500,7 @@
       <c r="D3" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>142</v>
       </c>
       <c r="F3" s="0" t="s">
@@ -2501,7 +2534,7 @@
       <c r="D4" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>147</v>
       </c>
       <c r="F4" s="0" t="s">
@@ -2580,7 +2613,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I12" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I12" type="list">
       <formula1>Comunas!$B$2:$B$40</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2592,7 +2625,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -2607,11 +2640,11 @@
   </sheetPr>
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="100.41"/>
   </cols>
@@ -2674,9 +2707,9 @@
         <f aca="false">VLOOKUP(I2,Q:R,2,0)</f>
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="str">
-        <f aca="false">VLOOKUP(J2,carreras!F:G,2,0)</f>
-        <v>1</v>
+      <c r="E2" s="8" t="e">
+        <f aca="false">VLOOKUP(J2,carreras!E:F,2,0)</f>
+        <v>#N/A</v>
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">VLOOKUP(K2,estudiantes!C:H,6,0)</f>
@@ -2701,9 +2734,9 @@
       <c r="L2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="M2" s="0" t="str">
+      <c r="M2" s="0" t="e">
         <f aca="false">_xlfn.CONCAT("INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), ",C2,", ",D2,", ",E2,", ",F2,", ",G2,");")</f>
-        <v>INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), 0, 1, 1, 1, 1);</v>
+        <v>#N/A</v>
       </c>
       <c r="Q2" s="0" t="s">
         <v>161</v>
@@ -2713,6 +2746,41 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">VLOOKUP(I3,Q:R,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E3" s="8" t="str">
+        <f aca="false">VLOOKUP(J3,carreras!E:F,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">VLOOKUP(K3,estudiantes!C:H,6,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">VLOOKUP(L3,niveles!B:D,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M3" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), ",C3,", ",D3,", ",E3,", ",F3,", ",G3,");")</f>
+        <v>INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), 0, 2, 2, 2, 1);</v>
+      </c>
       <c r="Q3" s="0" t="s">
         <v>163</v>
       </c>
@@ -2722,7 +2790,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q4" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="R4" s="0" t="n">
         <v>3</v>
@@ -2730,7 +2798,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q5" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="R5" s="0" t="n">
         <v>4</v>
@@ -2738,26 +2806,26 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I3" type="list">
       <formula1>matriculas!$Q$2:$Q$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2" type="list">
-      <formula1>carreras!$F$2:$F$16</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J3" type="list">
+      <formula1>carreras!$E$2:$E$16</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K2:K3" type="list">
       <formula1>estudiantes!$C$2:$C$19</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L3" type="list">
       <formula1>niveles!$B$2:$B$19</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -2770,13 +2838,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2786,26 +2854,26 @@
         <v>0</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>169</v>
+        <v>2</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>2</v>
+        <v>170</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>170</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>171</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -2817,24 +2885,105 @@
       <c r="D2" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(B2," - ",G2)</f>
+        <v>Ingenieria en Informatica - Tecnologia</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="F2" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(B2," - ",H2)</f>
-        <v>Ingenieria en Informatica - Bellavista</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="H2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>175</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(B3," - ",G3)</f>
+        <v>Tecnico en Administracion de Empresas - Negocios</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO carreras(nombre,codigo,escuela_id) VALUES ('",B3,"', '",C3,"', ",D3,");")</f>
+        <v>INSERT INTO carreras(nombre,codigo,escuela_id) VALUES ('Tecnico en Administracion de Empresas', 'TAD0001', 2);</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(B4," - ",G4)</f>
+        <v>Auditoria - Negocios</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="H4" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO carreras(nombre,codigo,escuela_id) VALUES ('",B4,"', '",C4,"', ",D4,");")</f>
+        <v>INSERT INTO carreras(nombre,codigo,escuela_id) VALUES ('Auditoria', 'AUD0001', 2);</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(B5," - ",G5)</f>
+        <v>Ingenieria en Negocios Electronicos - Negocios</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO carreras(nombre,codigo,escuela_id) VALUES ('",B5,"', '",C5,"', ",D5,");")</f>
+        <v>INSERT INTO carreras(nombre,codigo,escuela_id) VALUES ('Ingenieria en Negocios Electronicos', 'INE0001', 2);</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>

<commit_message>
query del 29 de sept
</commit_message>
<xml_diff>
--- a/Cargas Masivas.xlsx
+++ b/Cargas Masivas.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="217">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
@@ -477,6 +477,93 @@
     <t xml:space="preserve">Chacabuco 903</t>
   </si>
   <si>
+    <t xml:space="preserve">21800741-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manuel Soto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'2000-04-22'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msoto@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las Ardenas 1291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20800741-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'1999-10-23'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j.rosales@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carrera 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19800001-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luis Caceres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'1990-03-06'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lcaceres@yahoo.es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agustinas 1306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20800741-K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Torres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'2001-11-22'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mariatorres@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huerfanos 9999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22805741-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samuel Tapia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'2000-09-01'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stapia@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manuel Rodriguez 325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18800001-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oscar Maturana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'1998-04-15'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o.mat@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ohiggins 1593</t>
+  </si>
+  <si>
     <t xml:space="preserve">fecha_matricula</t>
   </si>
   <si>
@@ -528,7 +615,16 @@
     <t xml:space="preserve">TLP</t>
   </si>
   <si>
+    <t xml:space="preserve">Auditoria - Negocios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingenieria en Informatica - Tecnologia</t>
+  </si>
+  <si>
     <t xml:space="preserve">SP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingenieria en Negocios Electronicos - Negocios</t>
   </si>
   <si>
     <t xml:space="preserve">codigo</t>
@@ -672,7 +768,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -686,14 +782,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -729,10 +817,10 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="M4:M10 D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.84"/>
@@ -1017,10 +1105,10 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="1" sqref="M4:M10 E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="55.73"/>
@@ -1621,10 +1709,10 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="M4:M10 B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
   </cols>
@@ -1703,10 +1791,10 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="M4:M10 G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="33.29"/>
   </cols>
@@ -1777,13 +1865,13 @@
       <c r="H2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="5" t="str">
+      <c r="K2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(C2," - ",I2)</f>
         <v>Pablo Contreras -  Director(a) de Sede</v>
       </c>
@@ -1820,13 +1908,13 @@
       <c r="H3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="5" t="str">
+      <c r="K3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(C3," - ",I3)</f>
         <v>Laura Diaz -  Director(a) de Escuela</v>
       </c>
@@ -1863,13 +1951,13 @@
       <c r="H4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="5" t="str">
+      <c r="K4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(C4," - ",I4)</f>
         <v>Luis Mora -  Jefe(a) de Carrera</v>
       </c>
@@ -1906,13 +1994,13 @@
       <c r="H5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="5" t="str">
+      <c r="K5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(C5," - ",I5)</f>
         <v>Javiera Rosales -  Director(a) de Sede</v>
       </c>
@@ -1949,13 +2037,13 @@
       <c r="H6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="5" t="str">
+      <c r="K6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(C6," - ",I6)</f>
         <v>Lucia Suarez -  Director(a) de Escuela</v>
       </c>
@@ -1980,7 +2068,7 @@
       <c r="D7" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>101</v>
       </c>
       <c r="F7" s="0" t="s">
@@ -1994,13 +2082,13 @@
         <f aca="false">VLOOKUP(J7,Comunas!B:E,4,0)</f>
         <v>4</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="5" t="str">
+      <c r="K7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT(C7," - ",I7)</f>
         <v>Luis Ramirez -  Director(a) de Sede</v>
       </c>
@@ -2013,40 +2101,40 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I8" s="4"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I9" s="4"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="4"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="4"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I12" s="4"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I13" s="4"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I14" s="4"/>
+      <c r="I14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I15" s="4"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I16" s="4"/>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I17" s="4"/>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I18" s="4"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I19" s="4"/>
+      <c r="I19" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -2084,17 +2172,17 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="M4:M10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>61</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -2109,7 +2197,7 @@
       <c r="E1" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>61</v>
       </c>
       <c r="G1" s="0" t="s">
@@ -2123,7 +2211,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
+      <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -2138,7 +2226,7 @@
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="I2" s="0" t="str">
@@ -2147,7 +2235,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
+      <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -2162,7 +2250,7 @@
       <c r="E3" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="I3" s="0" t="str">
@@ -2185,10 +2273,10 @@
         <f aca="false">VLOOKUP(H4,Empleados!K:L,2,0)</f>
         <v>6</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="2" t="s">
         <v>112</v>
       </c>
       <c r="I4" s="0" t="str">
@@ -2225,10 +2313,10 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="M4:M10 D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="55.52"/>
   </cols>
@@ -2412,11 +2500,11 @@
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="M4:M10 A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="121.25"/>
   </cols>
@@ -2466,7 +2554,7 @@
       <c r="D2" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>137</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -2479,7 +2567,7 @@
       <c r="H2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="J2" s="0" t="str">
@@ -2500,7 +2588,7 @@
       <c r="D3" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>142</v>
       </c>
       <c r="F3" s="0" t="s">
@@ -2513,7 +2601,7 @@
       <c r="H3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J3" s="0" t="str">
@@ -2534,7 +2622,7 @@
       <c r="D4" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F4" s="0" t="s">
@@ -2547,7 +2635,7 @@
       <c r="H4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>59</v>
       </c>
       <c r="J4" s="0" t="str">
@@ -2556,60 +2644,214 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I5" s="4"/>
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">VLOOKUP(I5,Comunas!B:E,4,0)</f>
+        <v>4</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="J5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('",B5,"','",C5,"',",D5,",'",E5,"', '",F5,"',",G5,");")</f>
-        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('','',,'', '',);</v>
+        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('21800741-4','Manuel Soto','2000-04-22','msoto@gmail.com', 'Las Ardenas 1291',4);</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I6" s="4"/>
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">VLOOKUP(I6,Comunas!B:E,4,0)</f>
+        <v>2</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="J6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('",B6,"','",C6,"',",D6,",'",E6,"', '",F6,"',",G6,");")</f>
-        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('','',,'', '',);</v>
+        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('20800741-2','Javiera Rosales','1999-10-23','j.rosales@hotmail.com', 'Carrera 18',2);</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I7" s="4"/>
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">VLOOKUP(I7,Comunas!B:E,4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="J7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('",B7,"','",C7,"',",D7,",'",E7,"', '",F7,"',",G7,");")</f>
-        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('','',,'', '',);</v>
+        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('19800001-6','Luis Caceres','1990-03-06','lcaceres@yahoo.es', 'Agustinas 1306',1);</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I8" s="4"/>
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">VLOOKUP(I8,Comunas!B:E,4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="J8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('",B8,"','",C8,"',",D8,",'",E8,"', '",F8,"',",G8,");")</f>
-        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('','',,'', '',);</v>
+        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('20800741-K','Maria Torres','2001-11-22','mariatorres@gmail.com', 'Huerfanos 9999',1);</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I9" s="4"/>
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">VLOOKUP(I9,Comunas!B:E,4,0)</f>
+        <v>23</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('",B9,"','",C9,"',",D9,",'",E9,"', '",F9,"',",G9,");")</f>
-        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('','',,'', '',);</v>
+        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('22805741-8','Samuel Tapia','2000-09-01','stapia@gmail.com', 'Manuel Rodriguez 325',23);</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="4"/>
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">VLOOKUP(I10,Comunas!B:E,4,0)</f>
+        <v>3</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="J10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('",B10,"','",C10,"',",D10,",'",E10,"', '",F10,"',",G10,");")</f>
-        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('','',,'', '',);</v>
+        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('18800001-3','Oscar Maturana','1998-04-15','o.mat@hotmail.com', 'Ohiggins 1593',3);</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="4"/>
-      <c r="J11" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT("INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('",B11,"','",C11,"',",D11,",'",E11,"', '",F11,"',",G11,");")</f>
-        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('','',,'', '',);</v>
-      </c>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I12" s="4"/>
-      <c r="J12" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT("INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('",B12,"','",C12,"',",D12,",'",E12,"', '",F12,"',",G12,");")</f>
-        <v>INSERT INTO estudiantes(rut, nombre, fecha_nac, email, direccion, comuna_id) VALUES('','',,'', '',);</v>
-      </c>
+      <c r="I12" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2622,6 +2864,12 @@
     <hyperlink ref="E2" r:id="rId1" display="fperez@gmail.com"/>
     <hyperlink ref="E3" r:id="rId2" display="e.jara@hotmail.com"/>
     <hyperlink ref="E4" r:id="rId3" display="jmoraless@gmail.com"/>
+    <hyperlink ref="E5" r:id="rId4" display="msoto@gmail.com"/>
+    <hyperlink ref="E6" r:id="rId5" display="j.rosales@hotmail.com"/>
+    <hyperlink ref="E7" r:id="rId6" display="lcaceres@yahoo.es"/>
+    <hyperlink ref="E8" r:id="rId7" display="mariatorres@gmail.com"/>
+    <hyperlink ref="E9" r:id="rId8" display="stapia@gmail.com"/>
+    <hyperlink ref="E10" r:id="rId9" display="o.mat@hotmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2638,13 +2886,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
+      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4:M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="100.41"/>
   </cols>
@@ -2654,46 +2902,46 @@
         <v>2</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>151</v>
+        <v>180</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="M1" s="0" t="s">
         <v>3</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>160</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2707,7 +2955,7 @@
         <f aca="false">VLOOKUP(I2,Q:R,2,0)</f>
         <v>1</v>
       </c>
-      <c r="E2" s="8" t="e">
+      <c r="E2" s="6" t="e">
         <f aca="false">VLOOKUP(J2,carreras!E:F,2,0)</f>
         <v>#N/A</v>
       </c>
@@ -2720,18 +2968,19 @@
         <v>1</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="K2" s="4" t="s">
+        <f aca="false">A2</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>113</v>
       </c>
       <c r="M2" s="0" t="e">
@@ -2739,13 +2988,16 @@
         <v>#N/A</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>161</v>
+        <v>190</v>
       </c>
       <c r="R2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
       </c>
@@ -2753,7 +3005,7 @@
         <f aca="false">VLOOKUP(I3,Q:R,2,0)</f>
         <v>2</v>
       </c>
-      <c r="E3" s="8" t="str">
+      <c r="E3" s="6" t="str">
         <f aca="false">VLOOKUP(J3,carreras!E:F,2,0)</f>
         <v>2</v>
       </c>
@@ -2765,16 +3017,20 @@
         <f aca="false">VLOOKUP(L3,niveles!B:D,3,0)</f>
         <v>1</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="H3" s="0" t="n">
+        <f aca="false">A3</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="2" t="s">
         <v>113</v>
       </c>
       <c r="M3" s="0" t="str">
@@ -2782,43 +3038,326 @@
         <v>INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), 0, 2, 2, 2, 1);</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="R3" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="n">
+        <v>55000</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">VLOOKUP(I4,Q:R,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="6" t="str">
+        <f aca="false">VLOOKUP(J4,carreras!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">VLOOKUP(K4,estudiantes!C:H,6,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">VLOOKUP(L4,niveles!B:D,3,0)</f>
+        <v>3</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">A4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), ",C4,", ",D4,", ",E4,", ",F4,", ",G4,");")</f>
+        <v>INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), 55000, 3, 3, 3, 3);</v>
+      </c>
       <c r="Q4" s="0" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="R4" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="n">
+        <v>60000</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">VLOOKUP(I5,Q:R,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="6" t="str">
+        <f aca="false">VLOOKUP(J5,carreras!E:F,2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">VLOOKUP(K5,estudiantes!C:H,6,0)</f>
+        <v>6</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">VLOOKUP(L5,niveles!B:D,3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">A5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M5" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), ",C5,", ",D5,", ",E5,", ",F5,", ",G5,");")</f>
+        <v>INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), 60000, 2, 1, 6, 4);</v>
+      </c>
       <c r="Q5" s="0" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
       <c r="R5" s="0" t="n">
         <v>4</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="n">
+        <v>85000</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">VLOOKUP(I6,Q:R,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f aca="false">VLOOKUP(J6,carreras!E:F,2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <f aca="false">VLOOKUP(K6,estudiantes!C:H,6,0)</f>
+        <v>7</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">VLOOKUP(L6,niveles!B:D,3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">A6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), ",C6,", ",D6,", ",E6,", ",F6,", ",G6,");")</f>
+        <v>INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), 85000, 2, 4, 7, 2);</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="n">
+        <v>65000</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">VLOOKUP(I7,Q:R,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E7" s="6" t="str">
+        <f aca="false">VLOOKUP(J7,carreras!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <f aca="false">VLOOKUP(K7,estudiantes!C:H,6,0)</f>
+        <v>8</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">VLOOKUP(L7,niveles!B:D,3,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <f aca="false">A7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), ",C7,", ",D7,", ",E7,", ",F7,", ",G7,");")</f>
+        <v>INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), 65000, 2, 3, 8, 5);</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">VLOOKUP(I8,Q:R,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E8" s="6" t="str">
+        <f aca="false">VLOOKUP(J8,carreras!E:F,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <f aca="false">VLOOKUP(K8,estudiantes!C:H,6,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">VLOOKUP(L8,niveles!B:D,3,0)</f>
+        <v>6</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">A8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), ",C8,", ",D8,", ",E8,", ",F8,", ",G8,");")</f>
+        <v>INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), 0, 2, 2, 4, 6);</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">VLOOKUP(I9,Q:R,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f aca="false">VLOOKUP(J9,carreras!E:F,2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <f aca="false">VLOOKUP(K9,estudiantes!C:H,6,0)</f>
+        <v>9</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">VLOOKUP(L9,niveles!B:D,3,0)</f>
+        <v>7</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">A9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M9" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), ",C9,", ",D9,", ",E9,", ",F9,", ",G9,");")</f>
+        <v>INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), 120000, 2, 4, 9, 7);</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="n">
+        <v>45000</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">VLOOKUP(I10,Q:R,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E10" s="6" t="str">
+        <f aca="false">VLOOKUP(J10,carreras!E:F,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <f aca="false">VLOOKUP(K10,estudiantes!C:H,6,0)</f>
+        <v>5</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">VLOOKUP(L10,niveles!B:D,3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <f aca="false">A10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="M10" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), ",C10,", ",D10,", ",E10,", ",F10,", ",G10,");")</f>
+        <v>INSERT INTO matriculas (fecha_matricula, valor, regimen, carrera_id, estudiante_id, nivel_id) VALUES(now(), 45000, 2, 2, 5, 2);</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I3" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I10" type="list">
       <formula1>matriculas!$Q$2:$Q$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J3" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J10" type="list">
       <formula1>carreras!$E$2:$E$16</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K2:K3" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K2:K10" type="list">
       <formula1>estudiantes!$C$2:$C$19</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L3" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L10" type="list">
       <formula1>niveles!$B$2:$B$19</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2840,11 +3379,11 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="1" sqref="M4:M10 H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2854,57 +3393,57 @@
         <v>0</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>167</v>
+        <v>199</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>168</v>
+        <v>200</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>169</v>
+        <v>201</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>170</v>
+        <v>202</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>171</v>
+      <c r="A2" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>172</v>
+        <v>204</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>173</v>
+        <v>205</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>171</v>
+        <v>203</v>
       </c>
       <c r="E2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(B2," - ",G2)</f>
         <v>Ingenieria en Informatica - Tecnologia</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>171</v>
+      <c r="F2" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>175</v>
+      <c r="A3" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2</v>
@@ -2913,11 +3452,11 @@
         <f aca="false">_xlfn.CONCAT(B3," - ",G3)</f>
         <v>Tecnico en Administracion de Empresas - Negocios</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>175</v>
+      <c r="F3" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="H3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("INSERT INTO carreras(nombre,codigo,escuela_id) VALUES ('",B3,"', '",C3,"', ",D3,");")</f>
@@ -2925,14 +3464,14 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>179</v>
+      <c r="A4" s="6" t="s">
+        <v>211</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>180</v>
+        <v>212</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
@@ -2941,11 +3480,11 @@
         <f aca="false">_xlfn.CONCAT(B4," - ",G4)</f>
         <v>Auditoria - Negocios</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>179</v>
+      <c r="F4" s="6" t="s">
+        <v>211</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="H4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("INSERT INTO carreras(nombre,codigo,escuela_id) VALUES ('",B4,"', '",C4,"', ",D4,");")</f>
@@ -2953,14 +3492,14 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>182</v>
+      <c r="A5" s="6" t="s">
+        <v>214</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>2</v>
@@ -2969,11 +3508,11 @@
         <f aca="false">_xlfn.CONCAT(B5," - ",G5)</f>
         <v>Ingenieria en Negocios Electronicos - Negocios</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>182</v>
+      <c r="F5" s="6" t="s">
+        <v>214</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="H5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("INSERT INTO carreras(nombre,codigo,escuela_id) VALUES ('",B5,"', '",C5,"', ",D5,");")</f>

</xml_diff>